<commit_message>
“Continue with POC.” (plan of care)
</commit_message>
<xml_diff>
--- a/src/je/panse/doro/aeternum/dataxlsx/Plan9List.xlsx
+++ b/src/je/panse/doro/aeternum/dataxlsx/Plan9List.xlsx
@@ -21,21 +21,61 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="4">
-  <si>
-    <t xml:space="preserve">Obtain Glucose, HbA1c </t>
-  </si>
-  <si>
-    <t xml:space="preserve">increased hunger</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+  <si>
+    <t xml:space="preserve">Patient education, counseling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lab tests are needed to evaluate patient status today.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tests, procedures, other laboratory studies : </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specialist referral(s) or consults</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> “The client shows greater success with activates involving physical cueing.”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“Continue with POC.” (plan of care)</t>
   </si>
   <si>
     <t xml:space="preserve">.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buy fresh food often.
+Avoid  to “fast” foods, frozen dinners, and canned foods.
+Use spices, herbs, and sodium-free seasonings in place of salt. 
+Check for sodium on the Nutrition Facts label of food packages. 
+Rinse canned vegetables, beans, meats etc  before eating.
+Look for food labels with words like sodium free or salt free</t>
   </si>
   <si>
     <t xml:space="preserve">• Periarthritis shoulder – Pain and limitation of movements 
 • Cheiroarthropathy – Stiffness and limited mobility of fingers 
 • Neuroarthropathy • Painless unilateral swelling of foot and ankle 
 • Spinal hyperostosis – Mild back pain with preservation of back movements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weight loss of 5%-10%.  
+Reduction in fat intake &lt; 30% of calories.  
+Reduction in saturated fat intake &lt; 10% of calories.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your diet should contain less than 2,300 milligrams of sodium each day.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Increase in physical activity levels. 
+The brisk walking should last for at least 30 minutes 
+and should be undertaken  at least three times a week.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://owl.purdue.edu/owl/subject_specific_writing/healthcare_writing/soap_notes/soap_note_tips.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regular inspection and examination of the foot at risk.
+Appropriate footwear.</t>
   </si>
 </sst>
 </file>
@@ -136,13 +176,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="32.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="32.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="81.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.62"/>
@@ -160,44 +200,74 @@
     </row>
     <row r="3" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="114.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="64.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B10" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
@@ -220,7 +290,7 @@
       <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="36.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="36.578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E1" s="1"/>

</xml_diff>